<commit_message>
adding boardfiles for convenience
</commit_message>
<xml_diff>
--- a/Lab C/Outputs.xlsx
+++ b/Lab C/Outputs.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SODONNE8\Documents\GitHub\DIGITAL-SYSTEMS-DESIGN\Lab C\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shane\Documents\DIGITAL-SYSTEMS-DESIGN\Lab C\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{761DFEB8-CD38-4B4D-AFE7-B1D0FDADFD34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CDB50C7-0986-4374-87D9-BF80A2D244F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{025601DB-65F8-4BAF-A614-36994E3E5468}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{025601DB-65F8-4BAF-A614-36994E3E5468}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="29">
   <si>
     <t>X</t>
   </si>
@@ -75,6 +76,54 @@
   </si>
   <si>
     <t>"-32 - 1"</t>
+  </si>
+  <si>
+    <t>Test Vector ID</t>
+  </si>
+  <si>
+    <t>sel</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>c_out expected</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Overflow expected </t>
+  </si>
+  <si>
+    <t>Sum expected</t>
+  </si>
+  <si>
+    <t>6'b00_0100</t>
+  </si>
+  <si>
+    <t>6'b00_0001</t>
+  </si>
+  <si>
+    <t>6'b00_0000</t>
+  </si>
+  <si>
+    <t>6'b01_1111</t>
+  </si>
+  <si>
+    <t>6'b10_0000</t>
+  </si>
+  <si>
+    <t>6'b11_1111</t>
+  </si>
+  <si>
+    <t>6'b11_0000</t>
+  </si>
+  <si>
+    <t>6'b00_0101</t>
+  </si>
+  <si>
+    <t>6'b11_110</t>
   </si>
 </sst>
 </file>
@@ -110,7 +159,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -236,6 +285,180 @@
         <color indexed="64"/>
       </right>
       <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom style="medium">
@@ -248,7 +471,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -298,6 +521,45 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -685,17 +947,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B655FC1-2CEA-444B-B7FA-EFC488C6BD0E}">
   <dimension ref="B4:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView zoomScale="68" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="7" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="7" width="10.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="5" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B5" s="16"/>
       <c r="C5" s="1" t="s">
         <v>8</v>
@@ -713,7 +975,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B6" s="1" t="s">
         <v>0</v>
       </c>
@@ -733,7 +995,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B7" s="10" t="s">
         <v>1</v>
       </c>
@@ -753,7 +1015,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B8" s="4" t="s">
         <v>2</v>
       </c>
@@ -773,7 +1035,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:7" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B9" s="10" t="s">
         <v>3</v>
       </c>
@@ -793,11 +1055,175 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B10" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C37D4E4A-D892-4E78-B63E-43EFFD62BB37}">
+  <dimension ref="B2:H8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="8.7265625" style="18"/>
+    <col min="2" max="2" width="12.08984375" style="18" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.7265625" style="18"/>
+    <col min="4" max="5" width="10.54296875" style="18" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.1796875" style="18" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.1796875" style="18" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.1796875" style="18" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.7265625" style="18"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="3" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B3" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="H3" s="23" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B4" s="24">
+        <v>1</v>
+      </c>
+      <c r="C4" s="20">
+        <v>0</v>
+      </c>
+      <c r="D4" s="20" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" s="20">
+        <v>0</v>
+      </c>
+      <c r="G4" s="20">
+        <v>0</v>
+      </c>
+      <c r="H4" s="30" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B5" s="25">
+        <v>2</v>
+      </c>
+      <c r="C5" s="19">
+        <v>1</v>
+      </c>
+      <c r="D5" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" s="19">
+        <v>0</v>
+      </c>
+      <c r="G5" s="19">
+        <v>0</v>
+      </c>
+      <c r="H5" s="26" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B6" s="25">
+        <v>3</v>
+      </c>
+      <c r="C6" s="19">
+        <v>1</v>
+      </c>
+      <c r="D6" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" s="19">
+        <v>0</v>
+      </c>
+      <c r="G6" s="19">
+        <v>1</v>
+      </c>
+      <c r="H6" s="26" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B7" s="25">
+        <v>4</v>
+      </c>
+      <c r="C7" s="19">
+        <v>0</v>
+      </c>
+      <c r="D7" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" s="19">
+        <v>1</v>
+      </c>
+      <c r="G7" s="19">
+        <v>1</v>
+      </c>
+      <c r="H7" s="26" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B8" s="27">
+        <v>5</v>
+      </c>
+      <c r="C8" s="28">
+        <v>1</v>
+      </c>
+      <c r="D8" s="28" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" s="28" t="s">
+        <v>26</v>
+      </c>
+      <c r="F8" s="28">
+        <v>0</v>
+      </c>
+      <c r="G8" s="28">
+        <v>0</v>
+      </c>
+      <c r="H8" s="29" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>